<commit_message>
S&P 500 Realtime Excel File
</commit_message>
<xml_diff>
--- a/S&P Excel Files/SP500_Realtime_Excel.xlsx
+++ b/S&P Excel Files/SP500_Realtime_Excel.xlsx
@@ -531,7 +531,7 @@
         <v>-0.11</v>
       </c>
       <c r="J2" t="n">
-        <v>21126925</v>
+        <v>21241322</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -577,7 +577,7 @@
         <v>171</v>
       </c>
       <c r="I3" t="n">
-        <v>-3.18</v>
+        <v>-3.21</v>
       </c>
       <c r="J3" t="n">
         <v>105231182</v>
@@ -629,7 +629,7 @@
         <v>-0.9399999999999999</v>
       </c>
       <c r="J4" t="n">
-        <v>47709564</v>
+        <v>47818182</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -724,7 +724,7 @@
         <v>148</v>
       </c>
       <c r="I6" t="n">
-        <v>-1.06</v>
+        <v>-1.05</v>
       </c>
       <c r="J6" t="n">
         <v>19781751</v>
@@ -825,7 +825,7 @@
         <v>-1.35</v>
       </c>
       <c r="J8" t="n">
-        <v>9672486</v>
+        <v>9684867</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -874,7 +874,7 @@
         <v>-0.7</v>
       </c>
       <c r="J9" t="n">
-        <v>2495127</v>
+        <v>3385450</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -923,7 +923,7 @@
         <v>-0.48</v>
       </c>
       <c r="J10" t="n">
-        <v>2559490</v>
+        <v>3007197</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -963,13 +963,13 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="H11" t="n">
         <v>1348</v>
       </c>
       <c r="I11" t="n">
-        <v>1.58</v>
+        <v>1.48</v>
       </c>
       <c r="J11" t="n">
         <v>7207792</v>
@@ -1021,7 +1021,7 @@
         <v>0.14</v>
       </c>
       <c r="J12" t="n">
-        <v>3469584</v>
+        <v>5037911</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -1070,7 +1070,7 @@
         <v>1.29</v>
       </c>
       <c r="J13" t="n">
-        <v>7196951</v>
+        <v>10847445</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -1119,7 +1119,7 @@
         <v>-2.01</v>
       </c>
       <c r="J14" t="n">
-        <v>72354689</v>
+        <v>72890133</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1168,7 +1168,7 @@
         <v>0.28</v>
       </c>
       <c r="J15" t="n">
-        <v>9879027</v>
+        <v>13985913</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -1266,7 +1266,7 @@
         <v>-0.12</v>
       </c>
       <c r="J17" t="n">
-        <v>2515074</v>
+        <v>3661675</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
@@ -1315,7 +1315,7 @@
         <v>0.5</v>
       </c>
       <c r="J18" t="n">
-        <v>9011431</v>
+        <v>14640089</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -1364,7 +1364,7 @@
         <v>1.75</v>
       </c>
       <c r="J19" t="n">
-        <v>3116795</v>
+        <v>4179674</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
@@ -1462,7 +1462,7 @@
         <v>0.1</v>
       </c>
       <c r="J21" t="n">
-        <v>3839818</v>
+        <v>5890424</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -1511,7 +1511,7 @@
         <v>-1.16</v>
       </c>
       <c r="J22" t="n">
-        <v>15559458</v>
+        <v>17687153</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -1560,7 +1560,7 @@
         <v>-0.13</v>
       </c>
       <c r="J23" t="n">
-        <v>2082005</v>
+        <v>2082800</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -1609,7 +1609,7 @@
         <v>0.39</v>
       </c>
       <c r="J24" t="n">
-        <v>4135809</v>
+        <v>5722152</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -1658,7 +1658,7 @@
         <v>-0.06</v>
       </c>
       <c r="J25" t="n">
-        <v>4435792</v>
+        <v>7571504</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -1707,7 +1707,7 @@
         <v>0.15</v>
       </c>
       <c r="J26" t="n">
-        <v>4444001</v>
+        <v>6069900</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
@@ -1756,7 +1756,7 @@
         <v>1.57</v>
       </c>
       <c r="J27" t="n">
-        <v>37203894</v>
+        <v>42886384</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
@@ -1802,7 +1802,7 @@
         <v>178</v>
       </c>
       <c r="I28" t="n">
-        <v>-3.89</v>
+        <v>-3.92</v>
       </c>
       <c r="J28" t="n">
         <v>74478235</v>
@@ -1854,7 +1854,7 @@
         <v>-0.06</v>
       </c>
       <c r="J29" t="n">
-        <v>5422061</v>
+        <v>7871662</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -1952,7 +1952,7 @@
         <v>-0.15</v>
       </c>
       <c r="J31" t="n">
-        <v>8429779</v>
+        <v>12569627</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -1992,13 +1992,13 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H32" t="n">
         <v>172</v>
       </c>
       <c r="I32" t="n">
-        <v>0.31</v>
+        <v>0.26</v>
       </c>
       <c r="J32" t="n">
         <v>4318363</v>
@@ -2050,7 +2050,7 @@
         <v>-1.23</v>
       </c>
       <c r="J33" t="n">
-        <v>5196985</v>
+        <v>5199799</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -2099,7 +2099,7 @@
         <v>0.36</v>
       </c>
       <c r="J34" t="n">
-        <v>2360880</v>
+        <v>2493661</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
@@ -2148,7 +2148,7 @@
         <v>0.71</v>
       </c>
       <c r="J35" t="n">
-        <v>884713</v>
+        <v>1218812</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
@@ -2246,7 +2246,7 @@
         <v>-0.25</v>
       </c>
       <c r="J37" t="n">
-        <v>8263627</v>
+        <v>10290784</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
@@ -2295,7 +2295,7 @@
         <v>0.45</v>
       </c>
       <c r="J38" t="n">
-        <v>14905362</v>
+        <v>17988648</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -2344,7 +2344,7 @@
         <v>-0.34</v>
       </c>
       <c r="J39" t="n">
-        <v>2292507</v>
+        <v>3438488</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
@@ -2491,7 +2491,7 @@
         <v>1.16</v>
       </c>
       <c r="J42" t="n">
-        <v>5227925</v>
+        <v>6285825</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
@@ -2638,7 +2638,7 @@
         <v>0.73</v>
       </c>
       <c r="J45" t="n">
-        <v>1494680</v>
+        <v>2310885</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>1.93</v>
       </c>
       <c r="J47" t="n">
-        <v>1980073</v>
+        <v>2606949</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -2782,7 +2782,7 @@
         <v>42</v>
       </c>
       <c r="I48" t="n">
-        <v>-1.29</v>
+        <v>-1.33</v>
       </c>
       <c r="J48" t="n">
         <v>50228404</v>
@@ -2880,10 +2880,10 @@
         <v>210</v>
       </c>
       <c r="I50" t="n">
-        <v>-1.21</v>
+        <v>-1.2</v>
       </c>
       <c r="J50" t="n">
-        <v>6137545</v>
+        <v>6142896</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -2932,7 +2932,7 @@
         <v>1.05</v>
       </c>
       <c r="J51" t="n">
-        <v>12454209</v>
+        <v>21828726</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -2972,13 +2972,13 @@
         </is>
       </c>
       <c r="G52" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H52" t="n">
         <v>42</v>
       </c>
       <c r="I52" t="n">
-        <v>-0.21</v>
+        <v>-0.26</v>
       </c>
       <c r="J52" t="n">
         <v>18454163</v>
@@ -3030,7 +3030,7 @@
         <v>0.82</v>
       </c>
       <c r="J53" t="n">
-        <v>14784504</v>
+        <v>16171854</v>
       </c>
       <c r="K53" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
         <v>2.14</v>
       </c>
       <c r="J55" t="n">
-        <v>3279352</v>
+        <v>3809647</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>-0.87</v>
       </c>
       <c r="J56" t="n">
-        <v>1079137</v>
+        <v>1254732</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
@@ -3275,7 +3275,7 @@
         <v>-0.32</v>
       </c>
       <c r="J58" t="n">
-        <v>22104967</v>
+        <v>27834009</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
@@ -3324,7 +3324,7 @@
         <v>0.38</v>
       </c>
       <c r="J59" t="n">
-        <v>9491819</v>
+        <v>11759910</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
@@ -3373,7 +3373,7 @@
         <v>1.57</v>
       </c>
       <c r="J60" t="n">
-        <v>10801814</v>
+        <v>13478287</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
@@ -3422,7 +3422,7 @@
         <v>0.23</v>
       </c>
       <c r="J61" t="n">
-        <v>2708674</v>
+        <v>3197360</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
@@ -3569,7 +3569,7 @@
         <v>1.18</v>
       </c>
       <c r="J64" t="n">
-        <v>3825725</v>
+        <v>4908932</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
@@ -3765,7 +3765,7 @@
         <v>-0.13</v>
       </c>
       <c r="J68" t="n">
-        <v>684482</v>
+        <v>1339562</v>
       </c>
       <c r="K68" t="inlineStr">
         <is>
@@ -3814,7 +3814,7 @@
         <v>3.49</v>
       </c>
       <c r="J69" t="n">
-        <v>4087212</v>
+        <v>4590755</v>
       </c>
       <c r="K69" t="inlineStr">
         <is>
@@ -3863,7 +3863,7 @@
         <v>0.1</v>
       </c>
       <c r="J70" t="n">
-        <v>3908391</v>
+        <v>3908340</v>
       </c>
       <c r="K70" t="inlineStr">
         <is>
@@ -3961,7 +3961,7 @@
         <v>2.66</v>
       </c>
       <c r="J72" t="n">
-        <v>7552697</v>
+        <v>10373244</v>
       </c>
       <c r="K72" t="inlineStr">
         <is>
@@ -4010,7 +4010,7 @@
         <v>-0.05</v>
       </c>
       <c r="J73" t="n">
-        <v>1406569</v>
+        <v>1407270</v>
       </c>
       <c r="K73" t="inlineStr">
         <is>
@@ -4059,7 +4059,7 @@
         <v>1.22</v>
       </c>
       <c r="J74" t="n">
-        <v>1525573</v>
+        <v>2141193</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
@@ -4108,7 +4108,7 @@
         <v>-1.35</v>
       </c>
       <c r="J75" t="n">
-        <v>16216784</v>
+        <v>17906829</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
@@ -4157,7 +4157,7 @@
         <v>2.25</v>
       </c>
       <c r="J76" t="n">
-        <v>515101</v>
+        <v>637877</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
@@ -4255,7 +4255,7 @@
         <v>0.9</v>
       </c>
       <c r="J78" t="n">
-        <v>303779</v>
+        <v>304207</v>
       </c>
       <c r="K78" t="inlineStr">
         <is>
@@ -4402,7 +4402,7 @@
         <v>0.52</v>
       </c>
       <c r="J81" t="n">
-        <v>2775700</v>
+        <v>3396217</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
@@ -4451,7 +4451,7 @@
         <v>0.71</v>
       </c>
       <c r="J82" t="n">
-        <v>1959237</v>
+        <v>2861390</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
@@ -4500,7 +4500,7 @@
         <v>0.26</v>
       </c>
       <c r="J83" t="n">
-        <v>392109</v>
+        <v>512449</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -4549,7 +4549,7 @@
         <v>1.69</v>
       </c>
       <c r="J84" t="n">
-        <v>15708822</v>
+        <v>17678276</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
@@ -4647,7 +4647,7 @@
         <v>0.38</v>
       </c>
       <c r="J86" t="n">
-        <v>3505334</v>
+        <v>4946183</v>
       </c>
       <c r="K86" t="inlineStr">
         <is>
@@ -4696,7 +4696,7 @@
         <v>-0.19</v>
       </c>
       <c r="J87" t="n">
-        <v>4139118</v>
+        <v>6039434</v>
       </c>
       <c r="K87" t="inlineStr">
         <is>
@@ -4745,7 +4745,7 @@
         <v>0.95</v>
       </c>
       <c r="J88" t="n">
-        <v>1043460</v>
+        <v>1400794</v>
       </c>
       <c r="K88" t="inlineStr">
         <is>
@@ -4892,7 +4892,7 @@
         <v>0.41</v>
       </c>
       <c r="J91" t="n">
-        <v>709959</v>
+        <v>908316</v>
       </c>
       <c r="K91" t="inlineStr">
         <is>
@@ -4990,7 +4990,7 @@
         <v>-0.62</v>
       </c>
       <c r="J93" t="n">
-        <v>7633274</v>
+        <v>12558770</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
@@ -5039,7 +5039,7 @@
         <v>-0.5</v>
       </c>
       <c r="J94" t="n">
-        <v>2736817</v>
+        <v>2277418</v>
       </c>
       <c r="K94" t="inlineStr">
         <is>
@@ -5137,7 +5137,7 @@
         <v>0.19</v>
       </c>
       <c r="J96" t="n">
-        <v>1855673</v>
+        <v>1857712</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
@@ -5186,7 +5186,7 @@
         <v>-0.29</v>
       </c>
       <c r="J97" t="n">
-        <v>1330796</v>
+        <v>2161354</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
@@ -5235,7 +5235,7 @@
         <v>-0.11</v>
       </c>
       <c r="J98" t="n">
-        <v>837861</v>
+        <v>1210276</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -5284,7 +5284,7 @@
         <v>0.19</v>
       </c>
       <c r="J99" t="n">
-        <v>2457627</v>
+        <v>3399046</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -5333,7 +5333,7 @@
         <v>-0.41</v>
       </c>
       <c r="J100" t="n">
-        <v>6553289</v>
+        <v>7523614</v>
       </c>
       <c r="K100" t="inlineStr">
         <is>
@@ -5422,13 +5422,13 @@
         </is>
       </c>
       <c r="G102" t="n">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H102" t="n">
         <v>195</v>
       </c>
       <c r="I102" t="n">
-        <v>-0.4</v>
+        <v>-0.75</v>
       </c>
       <c r="J102" t="n">
         <v>3108959</v>
@@ -5529,7 +5529,7 @@
         <v>1.87</v>
       </c>
       <c r="J104" t="n">
-        <v>2421571</v>
+        <v>2915750</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -5569,16 +5569,16 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H105" t="n">
         <v>287</v>
       </c>
       <c r="I105" t="n">
-        <v>1.34</v>
+        <v>1.27</v>
       </c>
       <c r="J105" t="n">
-        <v>3807924</v>
+        <v>3814066</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
@@ -5627,7 +5627,7 @@
         <v>0.24</v>
       </c>
       <c r="J106" t="n">
-        <v>2507907</v>
+        <v>2931208</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
@@ -5676,7 +5676,7 @@
         <v>0.34</v>
       </c>
       <c r="J107" t="n">
-        <v>1753528</v>
+        <v>1760627</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -5823,7 +5823,7 @@
         <v>1.23</v>
       </c>
       <c r="J110" t="n">
-        <v>1083753</v>
+        <v>1288919</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
@@ -5869,7 +5869,7 @@
         <v>322</v>
       </c>
       <c r="I111" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="J111" t="n">
         <v>1853903</v>
@@ -5921,7 +5921,7 @@
         <v>-0.12</v>
       </c>
       <c r="J112" t="n">
-        <v>841802</v>
+        <v>1039247</v>
       </c>
       <c r="K112" t="inlineStr">
         <is>
@@ -5970,7 +5970,7 @@
         <v>0.26</v>
       </c>
       <c r="J113" t="n">
-        <v>1284536</v>
+        <v>1823933</v>
       </c>
       <c r="K113" t="inlineStr">
         <is>
@@ -6019,7 +6019,7 @@
         <v>0.54</v>
       </c>
       <c r="J114" t="n">
-        <v>894734</v>
+        <v>1160673</v>
       </c>
       <c r="K114" t="inlineStr">
         <is>
@@ -6068,7 +6068,7 @@
         <v>-1.62</v>
       </c>
       <c r="J115" t="n">
-        <v>288227</v>
+        <v>311480</v>
       </c>
       <c r="K115" t="inlineStr">
         <is>
@@ -6117,7 +6117,7 @@
         <v>0.27</v>
       </c>
       <c r="J116" t="n">
-        <v>11384496</v>
+        <v>18392100</v>
       </c>
       <c r="K116" t="inlineStr">
         <is>
@@ -6166,7 +6166,7 @@
         <v>1.27</v>
       </c>
       <c r="J117" t="n">
-        <v>2062420</v>
+        <v>2635702</v>
       </c>
       <c r="K117" t="inlineStr">
         <is>
@@ -6215,7 +6215,7 @@
         <v>-0.29</v>
       </c>
       <c r="J118" t="n">
-        <v>1897823</v>
+        <v>2621394</v>
       </c>
       <c r="K118" t="inlineStr">
         <is>
@@ -6264,7 +6264,7 @@
         <v>-0.07000000000000001</v>
       </c>
       <c r="J119" t="n">
-        <v>6449050</v>
+        <v>6259197</v>
       </c>
       <c r="K119" t="inlineStr">
         <is>
@@ -6313,7 +6313,7 @@
         <v>1.06</v>
       </c>
       <c r="J120" t="n">
-        <v>1439573</v>
+        <v>1529884</v>
       </c>
       <c r="K120" t="inlineStr">
         <is>
@@ -6362,7 +6362,7 @@
         <v>-0.71</v>
       </c>
       <c r="J121" t="n">
-        <v>770528</v>
+        <v>1045946</v>
       </c>
       <c r="K121" t="inlineStr">
         <is>
@@ -6411,7 +6411,7 @@
         <v>-2.55</v>
       </c>
       <c r="J122" t="n">
-        <v>3657357</v>
+        <v>4339726</v>
       </c>
       <c r="K122" t="inlineStr">
         <is>
@@ -6509,7 +6509,7 @@
         <v>-0.77</v>
       </c>
       <c r="J124" t="n">
-        <v>1853257</v>
+        <v>2581083</v>
       </c>
       <c r="K124" t="inlineStr">
         <is>
@@ -6558,7 +6558,7 @@
         <v>0.13</v>
       </c>
       <c r="J125" t="n">
-        <v>10499272</v>
+        <v>10512289</v>
       </c>
       <c r="K125" t="inlineStr">
         <is>
@@ -6656,7 +6656,7 @@
         <v>-0.5600000000000001</v>
       </c>
       <c r="J127" t="n">
-        <v>2156718</v>
+        <v>2735229</v>
       </c>
       <c r="K127" t="inlineStr">
         <is>
@@ -6705,7 +6705,7 @@
         <v>0.14</v>
       </c>
       <c r="J128" t="n">
-        <v>2030021</v>
+        <v>2664739</v>
       </c>
       <c r="K128" t="inlineStr">
         <is>
@@ -6754,7 +6754,7 @@
         <v>0.48</v>
       </c>
       <c r="J129" t="n">
-        <v>2542791</v>
+        <v>3279393</v>
       </c>
       <c r="K129" t="inlineStr">
         <is>
@@ -6852,7 +6852,7 @@
         <v>1.9</v>
       </c>
       <c r="J131" t="n">
-        <v>501548</v>
+        <v>616051</v>
       </c>
       <c r="K131" t="inlineStr">
         <is>
@@ -6901,7 +6901,7 @@
         <v>0.57</v>
       </c>
       <c r="J132" t="n">
-        <v>1195107</v>
+        <v>1672548</v>
       </c>
       <c r="K132" t="inlineStr">
         <is>
@@ -6999,7 +6999,7 @@
         <v>0.79</v>
       </c>
       <c r="J134" t="n">
-        <v>391497</v>
+        <v>495505</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -7048,7 +7048,7 @@
         <v>-0.9399999999999999</v>
       </c>
       <c r="J135" t="n">
-        <v>680750</v>
+        <v>791075</v>
       </c>
       <c r="K135" t="inlineStr">
         <is>
@@ -7146,7 +7146,7 @@
         <v>1.6</v>
       </c>
       <c r="J137" t="n">
-        <v>6582385</v>
+        <v>8525127</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
@@ -7195,7 +7195,7 @@
         <v>1.51</v>
       </c>
       <c r="J138" t="n">
-        <v>863366</v>
+        <v>1071436</v>
       </c>
       <c r="K138" t="inlineStr">
         <is>
@@ -7244,7 +7244,7 @@
         <v>1.16</v>
       </c>
       <c r="J139" t="n">
-        <v>425069</v>
+        <v>427341</v>
       </c>
       <c r="K139" t="inlineStr">
         <is>
@@ -7391,7 +7391,7 @@
         <v>0.05</v>
       </c>
       <c r="J142" t="n">
-        <v>1994726</v>
+        <v>2481659</v>
       </c>
       <c r="K142" t="inlineStr">
         <is>
@@ -7440,7 +7440,7 @@
         <v>-0.32</v>
       </c>
       <c r="J143" t="n">
-        <v>14457940</v>
+        <v>16785583</v>
       </c>
       <c r="K143" t="inlineStr">
         <is>
@@ -7489,7 +7489,7 @@
         <v>2.04</v>
       </c>
       <c r="J144" t="n">
-        <v>4067501</v>
+        <v>4067299</v>
       </c>
       <c r="K144" t="inlineStr">
         <is>
@@ -7538,7 +7538,7 @@
         <v>0.01</v>
       </c>
       <c r="J145" t="n">
-        <v>956016</v>
+        <v>1289166</v>
       </c>
       <c r="K145" t="inlineStr">
         <is>
@@ -7734,7 +7734,7 @@
         <v>0.11</v>
       </c>
       <c r="J149" t="n">
-        <v>1497019</v>
+        <v>2410693</v>
       </c>
       <c r="K149" t="inlineStr">
         <is>
@@ -7832,7 +7832,7 @@
         <v>2.06</v>
       </c>
       <c r="J151" t="n">
-        <v>2094794</v>
+        <v>2472432</v>
       </c>
       <c r="K151" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
         <v>59</v>
       </c>
       <c r="I152" t="n">
-        <v>-0.68</v>
+        <v>-0.6</v>
       </c>
       <c r="J152" t="n">
         <v>3103991</v>
@@ -7979,7 +7979,7 @@
         <v>0.92</v>
       </c>
       <c r="J154" t="n">
-        <v>583503</v>
+        <v>721005</v>
       </c>
       <c r="K154" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
         <v>-0.3</v>
       </c>
       <c r="J155" t="n">
-        <v>4567646</v>
+        <v>5868459</v>
       </c>
       <c r="K155" t="inlineStr">
         <is>
@@ -8077,7 +8077,7 @@
         <v>-0.05</v>
       </c>
       <c r="J156" t="n">
-        <v>355881</v>
+        <v>424138</v>
       </c>
       <c r="K156" t="inlineStr">
         <is>
@@ -8126,7 +8126,7 @@
         <v>0.61</v>
       </c>
       <c r="J157" t="n">
-        <v>1228095</v>
+        <v>1825408</v>
       </c>
       <c r="K157" t="inlineStr">
         <is>
@@ -8175,7 +8175,7 @@
         <v>-0.25</v>
       </c>
       <c r="J158" t="n">
-        <v>1077980</v>
+        <v>1445297</v>
       </c>
       <c r="K158" t="inlineStr">
         <is>
@@ -8224,7 +8224,7 @@
         <v>-1.69</v>
       </c>
       <c r="J159" t="n">
-        <v>1233589</v>
+        <v>1455093</v>
       </c>
       <c r="K159" t="inlineStr">
         <is>
@@ -8273,7 +8273,7 @@
         <v>0.76</v>
       </c>
       <c r="J160" t="n">
-        <v>245389</v>
+        <v>402555</v>
       </c>
       <c r="K160" t="inlineStr">
         <is>
@@ -8322,7 +8322,7 @@
         <v>0.83</v>
       </c>
       <c r="J161" t="n">
-        <v>2859614</v>
+        <v>3602267</v>
       </c>
       <c r="K161" t="inlineStr">
         <is>
@@ -8420,7 +8420,7 @@
         <v>0.36</v>
       </c>
       <c r="J163" t="n">
-        <v>2854225</v>
+        <v>3671623</v>
       </c>
       <c r="K163" t="inlineStr">
         <is>
@@ -8469,7 +8469,7 @@
         <v>0.11</v>
       </c>
       <c r="J164" t="n">
-        <v>4645429</v>
+        <v>5363430</v>
       </c>
       <c r="K164" t="inlineStr">
         <is>
@@ -8616,7 +8616,7 @@
         <v>-0.2</v>
       </c>
       <c r="J167" t="n">
-        <v>5812753</v>
+        <v>5823350</v>
       </c>
       <c r="K167" t="inlineStr">
         <is>
@@ -8665,7 +8665,7 @@
         <v>0.36</v>
       </c>
       <c r="J168" t="n">
-        <v>1968156</v>
+        <v>2308841</v>
       </c>
       <c r="K168" t="inlineStr">
         <is>
@@ -8711,10 +8711,10 @@
         <v>971</v>
       </c>
       <c r="I169" t="n">
-        <v>3.54</v>
+        <v>3.58</v>
       </c>
       <c r="J169" t="n">
-        <v>8486589</v>
+        <v>8511885</v>
       </c>
       <c r="K169" t="inlineStr">
         <is>
@@ -8812,7 +8812,7 @@
         <v>1.2</v>
       </c>
       <c r="J171" t="n">
-        <v>5455966</v>
+        <v>5022250</v>
       </c>
       <c r="K171" t="inlineStr">
         <is>
@@ -8861,7 +8861,7 @@
         <v>0.59</v>
       </c>
       <c r="J172" t="n">
-        <v>1779268</v>
+        <v>2154663</v>
       </c>
       <c r="K172" t="inlineStr">
         <is>
@@ -8910,7 +8910,7 @@
         <v>-0.42</v>
       </c>
       <c r="J173" t="n">
-        <v>1130453</v>
+        <v>1459472</v>
       </c>
       <c r="K173" t="inlineStr">
         <is>
@@ -8959,7 +8959,7 @@
         <v>-0.48</v>
       </c>
       <c r="J174" t="n">
-        <v>2451789</v>
+        <v>2998868</v>
       </c>
       <c r="K174" t="inlineStr">
         <is>
@@ -9008,7 +9008,7 @@
         <v>-0.28</v>
       </c>
       <c r="J175" t="n">
-        <v>2602754</v>
+        <v>3533781</v>
       </c>
       <c r="K175" t="inlineStr">
         <is>
@@ -9106,7 +9106,7 @@
         <v>-0.85</v>
       </c>
       <c r="J177" t="n">
-        <v>1233542</v>
+        <v>1448938</v>
       </c>
       <c r="K177" t="inlineStr">
         <is>
@@ -9155,7 +9155,7 @@
         <v>-1.54</v>
       </c>
       <c r="J178" t="n">
-        <v>2169541</v>
+        <v>2328485</v>
       </c>
       <c r="K178" t="inlineStr">
         <is>
@@ -9204,7 +9204,7 @@
         <v>-0.01</v>
       </c>
       <c r="J179" t="n">
-        <v>3693949</v>
+        <v>3710921</v>
       </c>
       <c r="K179" t="inlineStr">
         <is>
@@ -9253,7 +9253,7 @@
         <v>0.7</v>
       </c>
       <c r="J180" t="n">
-        <v>901188</v>
+        <v>1343704</v>
       </c>
       <c r="K180" t="inlineStr">
         <is>
@@ -9351,7 +9351,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>47592540</v>
+        <v>54429987</v>
       </c>
       <c r="K182" t="inlineStr">
         <is>
@@ -9400,7 +9400,7 @@
         <v>2.78</v>
       </c>
       <c r="J183" t="n">
-        <v>13555782</v>
+        <v>12133400</v>
       </c>
       <c r="K183" t="inlineStr">
         <is>
@@ -9449,7 +9449,7 @@
         <v>1.03</v>
       </c>
       <c r="J184" t="n">
-        <v>155797</v>
+        <v>200312</v>
       </c>
       <c r="K184" t="inlineStr">
         <is>
@@ -9498,7 +9498,7 @@
         <v>1.16</v>
       </c>
       <c r="J185" t="n">
-        <v>10743420</v>
+        <v>15059903</v>
       </c>
       <c r="K185" t="inlineStr">
         <is>
@@ -9547,7 +9547,7 @@
         <v>-0.61</v>
       </c>
       <c r="J186" t="n">
-        <v>445445</v>
+        <v>627801</v>
       </c>
       <c r="K186" t="inlineStr">
         <is>
@@ -9645,7 +9645,7 @@
         <v>0.32</v>
       </c>
       <c r="J188" t="n">
-        <v>744694</v>
+        <v>896496</v>
       </c>
       <c r="K188" t="inlineStr">
         <is>
@@ -9792,7 +9792,7 @@
         <v>0.2</v>
       </c>
       <c r="J191" t="n">
-        <v>452890</v>
+        <v>591625</v>
       </c>
       <c r="K191" t="inlineStr">
         <is>
@@ -9841,7 +9841,7 @@
         <v>0.18</v>
       </c>
       <c r="J192" t="n">
-        <v>578663</v>
+        <v>765886</v>
       </c>
       <c r="K192" t="inlineStr">
         <is>
@@ -9939,7 +9939,7 @@
         <v>0.71</v>
       </c>
       <c r="J194" t="n">
-        <v>1124772</v>
+        <v>1588866</v>
       </c>
       <c r="K194" t="inlineStr">
         <is>
@@ -9988,7 +9988,7 @@
         <v>1.13</v>
       </c>
       <c r="J195" t="n">
-        <v>9393247</v>
+        <v>11589925</v>
       </c>
       <c r="K195" t="inlineStr">
         <is>
@@ -10037,7 +10037,7 @@
         <v>0.46</v>
       </c>
       <c r="J196" t="n">
-        <v>1943462</v>
+        <v>2779485</v>
       </c>
       <c r="K196" t="inlineStr">
         <is>
@@ -10086,7 +10086,7 @@
         <v>0.17</v>
       </c>
       <c r="J197" t="n">
-        <v>819225</v>
+        <v>995993</v>
       </c>
       <c r="K197" t="inlineStr">
         <is>
@@ -10135,7 +10135,7 @@
         <v>-0.03</v>
       </c>
       <c r="J198" t="n">
-        <v>1696259</v>
+        <v>1888331</v>
       </c>
       <c r="K198" t="inlineStr">
         <is>
@@ -10184,7 +10184,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="J199" t="n">
-        <v>1530602</v>
+        <v>1790555</v>
       </c>
       <c r="K199" t="inlineStr">
         <is>
@@ -10233,7 +10233,7 @@
         <v>-0.32</v>
       </c>
       <c r="J200" t="n">
-        <v>4277658</v>
+        <v>4948938</v>
       </c>
       <c r="K200" t="inlineStr">
         <is>
@@ -10282,7 +10282,7 @@
         <v>-1.36</v>
       </c>
       <c r="J201" t="n">
-        <v>1672379</v>
+        <v>2804270</v>
       </c>
       <c r="K201" t="inlineStr">
         <is>
@@ -10328,7 +10328,7 @@
         <v>78</v>
       </c>
       <c r="I202" t="n">
-        <v>1.03</v>
+        <v>1.06</v>
       </c>
       <c r="J202" t="n">
         <v>3053541</v>
@@ -10380,7 +10380,7 @@
         <v>0.6</v>
       </c>
       <c r="J203" t="n">
-        <v>412191</v>
+        <v>493319</v>
       </c>
       <c r="K203" t="inlineStr">
         <is>
@@ -10429,7 +10429,7 @@
         <v>-1.16</v>
       </c>
       <c r="J204" t="n">
-        <v>1847918</v>
+        <v>2238176</v>
       </c>
       <c r="K204" t="inlineStr">
         <is>
@@ -10478,7 +10478,7 @@
         <v>0.93</v>
       </c>
       <c r="J205" t="n">
-        <v>2600906</v>
+        <v>3178906</v>
       </c>
       <c r="K205" t="inlineStr">
         <is>
@@ -10576,7 +10576,7 @@
         <v>0.23</v>
       </c>
       <c r="J207" t="n">
-        <v>1968630</v>
+        <v>2570903</v>
       </c>
       <c r="K207" t="inlineStr">
         <is>
@@ -10625,7 +10625,7 @@
         <v>0.75</v>
       </c>
       <c r="J208" t="n">
-        <v>3676701</v>
+        <v>4182327</v>
       </c>
       <c r="K208" t="inlineStr">
         <is>
@@ -10723,7 +10723,7 @@
         <v>0.18</v>
       </c>
       <c r="J210" t="n">
-        <v>3100693</v>
+        <v>3107748</v>
       </c>
       <c r="K210" t="inlineStr">
         <is>
@@ -10867,7 +10867,7 @@
         <v>35</v>
       </c>
       <c r="I213" t="n">
-        <v>0.46</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="J213" t="n">
         <v>7373341</v>
@@ -10968,7 +10968,7 @@
         <v>1.42</v>
       </c>
       <c r="J215" t="n">
-        <v>11976557</v>
+        <v>13749010</v>
       </c>
       <c r="K215" t="inlineStr">
         <is>
@@ -11017,7 +11017,7 @@
         <v>0.19</v>
       </c>
       <c r="J216" t="n">
-        <v>838444</v>
+        <v>1036781</v>
       </c>
       <c r="K216" t="inlineStr">
         <is>
@@ -11066,7 +11066,7 @@
         <v>1.29</v>
       </c>
       <c r="J217" t="n">
-        <v>1227640</v>
+        <v>1835579</v>
       </c>
       <c r="K217" t="inlineStr">
         <is>
@@ -11115,7 +11115,7 @@
         <v>-0.01</v>
       </c>
       <c r="J218" t="n">
-        <v>1187396</v>
+        <v>1191345</v>
       </c>
       <c r="K218" t="inlineStr">
         <is>
@@ -11164,7 +11164,7 @@
         <v>0.63</v>
       </c>
       <c r="J219" t="n">
-        <v>1316334</v>
+        <v>1794795</v>
       </c>
       <c r="K219" t="inlineStr">
         <is>
@@ -11213,7 +11213,7 @@
         <v>-0.1</v>
       </c>
       <c r="J220" t="n">
-        <v>896297</v>
+        <v>1287247</v>
       </c>
       <c r="K220" t="inlineStr">
         <is>
@@ -11262,7 +11262,7 @@
         <v>1.86</v>
       </c>
       <c r="J221" t="n">
-        <v>4002199</v>
+        <v>5114151</v>
       </c>
       <c r="K221" t="inlineStr">
         <is>
@@ -11311,7 +11311,7 @@
         <v>-0.08</v>
       </c>
       <c r="J222" t="n">
-        <v>1045434</v>
+        <v>1375262</v>
       </c>
       <c r="K222" t="inlineStr">
         <is>
@@ -11357,7 +11357,7 @@
         <v>91</v>
       </c>
       <c r="I223" t="n">
-        <v>-0.2</v>
+        <v>-0.05</v>
       </c>
       <c r="J223" t="n">
         <v>2244227</v>
@@ -11409,7 +11409,7 @@
         <v>-0.05</v>
       </c>
       <c r="J224" t="n">
-        <v>2281332</v>
+        <v>2824821</v>
       </c>
       <c r="K224" t="inlineStr">
         <is>
@@ -11458,7 +11458,7 @@
         <v>0.16</v>
       </c>
       <c r="J225" t="n">
-        <v>5132364</v>
+        <v>7031843</v>
       </c>
       <c r="K225" t="inlineStr">
         <is>
@@ -11507,7 +11507,7 @@
         <v>-0.97</v>
       </c>
       <c r="J226" t="n">
-        <v>4765788</v>
+        <v>5858378</v>
       </c>
       <c r="K226" t="inlineStr">
         <is>
@@ -11556,7 +11556,7 @@
         <v>0.93</v>
       </c>
       <c r="J227" t="n">
-        <v>1871116</v>
+        <v>2330264</v>
       </c>
       <c r="K227" t="inlineStr">
         <is>
@@ -11605,7 +11605,7 @@
         <v>0.54</v>
       </c>
       <c r="J228" t="n">
-        <v>1853492</v>
+        <v>2280381</v>
       </c>
       <c r="K228" t="inlineStr">
         <is>
@@ -11654,7 +11654,7 @@
         <v>0.82</v>
       </c>
       <c r="J229" t="n">
-        <v>1167913</v>
+        <v>1580276</v>
       </c>
       <c r="K229" t="inlineStr">
         <is>
@@ -11703,7 +11703,7 @@
         <v>0.52</v>
       </c>
       <c r="J230" t="n">
-        <v>4070137</v>
+        <v>5024304</v>
       </c>
       <c r="K230" t="inlineStr">
         <is>
@@ -11752,7 +11752,7 @@
         <v>0.16</v>
       </c>
       <c r="J231" t="n">
-        <v>1071964</v>
+        <v>1240237</v>
       </c>
       <c r="K231" t="inlineStr">
         <is>
@@ -11801,7 +11801,7 @@
         <v>0.33</v>
       </c>
       <c r="J232" t="n">
-        <v>11576031</v>
+        <v>13186792</v>
       </c>
       <c r="K232" t="inlineStr">
         <is>
@@ -11948,7 +11948,7 @@
         <v>-1.2</v>
       </c>
       <c r="J235" t="n">
-        <v>10619304</v>
+        <v>11908351</v>
       </c>
       <c r="K235" t="inlineStr">
         <is>
@@ -11994,7 +11994,7 @@
         <v>104</v>
       </c>
       <c r="I236" t="n">
-        <v>-0.25</v>
+        <v>-0.39</v>
       </c>
       <c r="J236" t="n">
         <v>2191425</v>
@@ -12046,7 +12046,7 @@
         <v>1.18</v>
       </c>
       <c r="J237" t="n">
-        <v>3082915</v>
+        <v>8453924</v>
       </c>
       <c r="K237" t="inlineStr">
         <is>
@@ -12095,7 +12095,7 @@
         <v>1.42</v>
       </c>
       <c r="J238" t="n">
-        <v>15487498</v>
+        <v>17183864</v>
       </c>
       <c r="K238" t="inlineStr">
         <is>
@@ -12144,7 +12144,7 @@
         <v>-0.07000000000000001</v>
       </c>
       <c r="J239" t="n">
-        <v>1780151</v>
+        <v>2462624</v>
       </c>
       <c r="K239" t="inlineStr">
         <is>
@@ -12193,7 +12193,7 @@
         <v>-1.01</v>
       </c>
       <c r="J240" t="n">
-        <v>5020533</v>
+        <v>4861261</v>
       </c>
       <c r="K240" t="inlineStr">
         <is>
@@ -12242,7 +12242,7 @@
         <v>0.27</v>
       </c>
       <c r="J241" t="n">
-        <v>1136976</v>
+        <v>1501422</v>
       </c>
       <c r="K241" t="inlineStr">
         <is>
@@ -12291,7 +12291,7 @@
         <v>1.06</v>
       </c>
       <c r="J242" t="n">
-        <v>2006175</v>
+        <v>2334143</v>
       </c>
       <c r="K242" t="inlineStr">
         <is>
@@ -12340,7 +12340,7 @@
         <v>-0.8100000000000001</v>
       </c>
       <c r="J243" t="n">
-        <v>2394014</v>
+        <v>2891939</v>
       </c>
       <c r="K243" t="inlineStr">
         <is>
@@ -12389,7 +12389,7 @@
         <v>1.1</v>
       </c>
       <c r="J244" t="n">
-        <v>256195</v>
+        <v>346845</v>
       </c>
       <c r="K244" t="inlineStr">
         <is>
@@ -12438,7 +12438,7 @@
         <v>0.05</v>
       </c>
       <c r="J245" t="n">
-        <v>332416</v>
+        <v>430410</v>
       </c>
       <c r="K245" t="inlineStr">
         <is>
@@ -12487,7 +12487,7 @@
         <v>1.61</v>
       </c>
       <c r="J246" t="n">
-        <v>784082</v>
+        <v>973898</v>
       </c>
       <c r="K246" t="inlineStr">
         <is>
@@ -12536,7 +12536,7 @@
         <v>1.06</v>
       </c>
       <c r="J247" t="n">
-        <v>6609686</v>
+        <v>6612688</v>
       </c>
       <c r="K247" t="inlineStr">
         <is>
@@ -12585,7 +12585,7 @@
         <v>1.15</v>
       </c>
       <c r="J248" t="n">
-        <v>696862</v>
+        <v>1033398</v>
       </c>
       <c r="K248" t="inlineStr">
         <is>
@@ -12781,7 +12781,7 @@
         <v>-0.73</v>
       </c>
       <c r="J252" t="n">
-        <v>2651234</v>
+        <v>2601789</v>
       </c>
       <c r="K252" t="inlineStr">
         <is>
@@ -12879,7 +12879,7 @@
         <v>0.76</v>
       </c>
       <c r="J254" t="n">
-        <v>2280237</v>
+        <v>2241959</v>
       </c>
       <c r="K254" t="inlineStr">
         <is>
@@ -12928,7 +12928,7 @@
         <v>0.47</v>
       </c>
       <c r="J255" t="n">
-        <v>3846027</v>
+        <v>5044091</v>
       </c>
       <c r="K255" t="inlineStr">
         <is>
@@ -12977,7 +12977,7 @@
         <v>0.7</v>
       </c>
       <c r="J256" t="n">
-        <v>688546</v>
+        <v>688946</v>
       </c>
       <c r="K256" t="inlineStr">
         <is>
@@ -13026,7 +13026,7 @@
         <v>0.93</v>
       </c>
       <c r="J257" t="n">
-        <v>5908691</v>
+        <v>5912262</v>
       </c>
       <c r="K257" t="inlineStr">
         <is>
@@ -13124,7 +13124,7 @@
         <v>-0.99</v>
       </c>
       <c r="J259" t="n">
-        <v>1560916</v>
+        <v>1804218</v>
       </c>
       <c r="K259" t="inlineStr">
         <is>
@@ -13222,7 +13222,7 @@
         <v>0.76</v>
       </c>
       <c r="J261" t="n">
-        <v>1043077</v>
+        <v>1290657</v>
       </c>
       <c r="K261" t="inlineStr">
         <is>
@@ -13271,7 +13271,7 @@
         <v>2.28</v>
       </c>
       <c r="J262" t="n">
-        <v>1017645</v>
+        <v>1154691</v>
       </c>
       <c r="K262" t="inlineStr">
         <is>
@@ -13320,7 +13320,7 @@
         <v>-0.26</v>
       </c>
       <c r="J263" t="n">
-        <v>795016</v>
+        <v>940564</v>
       </c>
       <c r="K263" t="inlineStr">
         <is>
@@ -13369,7 +13369,7 @@
         <v>-1.45</v>
       </c>
       <c r="J264" t="n">
-        <v>1163409</v>
+        <v>1405450</v>
       </c>
       <c r="K264" t="inlineStr">
         <is>
@@ -13565,7 +13565,7 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="J268" t="n">
-        <v>1611856</v>
+        <v>1571833</v>
       </c>
       <c r="K268" t="inlineStr">
         <is>
@@ -13663,7 +13663,7 @@
         <v>-0.5600000000000001</v>
       </c>
       <c r="J270" t="n">
-        <v>1902401</v>
+        <v>2431059</v>
       </c>
       <c r="K270" t="inlineStr">
         <is>
@@ -13712,7 +13712,7 @@
         <v>1.69</v>
       </c>
       <c r="J271" t="n">
-        <v>135110</v>
+        <v>131567</v>
       </c>
       <c r="K271" t="inlineStr">
         <is>
@@ -13761,7 +13761,7 @@
         <v>0.61</v>
       </c>
       <c r="J272" t="n">
-        <v>708878</v>
+        <v>936693</v>
       </c>
       <c r="K272" t="inlineStr">
         <is>
@@ -13810,7 +13810,7 @@
         <v>0.64</v>
       </c>
       <c r="J273" t="n">
-        <v>1356938</v>
+        <v>1781927</v>
       </c>
       <c r="K273" t="inlineStr">
         <is>
@@ -13859,7 +13859,7 @@
         <v>0.57</v>
       </c>
       <c r="J274" t="n">
-        <v>1141437</v>
+        <v>1340340</v>
       </c>
       <c r="K274" t="inlineStr">
         <is>
@@ -13908,7 +13908,7 @@
         <v>-0.21</v>
       </c>
       <c r="J275" t="n">
-        <v>5064096</v>
+        <v>6666084</v>
       </c>
       <c r="K275" t="inlineStr">
         <is>
@@ -13957,7 +13957,7 @@
         <v>-0.66</v>
       </c>
       <c r="J276" t="n">
-        <v>1420709</v>
+        <v>1787470</v>
       </c>
       <c r="K276" t="inlineStr">
         <is>
@@ -14006,7 +14006,7 @@
         <v>0.86</v>
       </c>
       <c r="J277" t="n">
-        <v>4009090</v>
+        <v>5198571</v>
       </c>
       <c r="K277" t="inlineStr">
         <is>
@@ -14104,7 +14104,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="J279" t="n">
-        <v>2319905</v>
+        <v>2740010</v>
       </c>
       <c r="K279" t="inlineStr">
         <is>
@@ -14202,7 +14202,7 @@
         <v>-0.58</v>
       </c>
       <c r="J281" t="n">
-        <v>1549008</v>
+        <v>1861281</v>
       </c>
       <c r="K281" t="inlineStr">
         <is>
@@ -14251,7 +14251,7 @@
         <v>1.1</v>
       </c>
       <c r="J282" t="n">
-        <v>8341990</v>
+        <v>9852879</v>
       </c>
       <c r="K282" t="inlineStr">
         <is>
@@ -14300,7 +14300,7 @@
         <v>0.77</v>
       </c>
       <c r="J283" t="n">
-        <v>5327564</v>
+        <v>6695747</v>
       </c>
       <c r="K283" t="inlineStr">
         <is>
@@ -14398,7 +14398,7 @@
         <v>0</v>
       </c>
       <c r="J285" t="n">
-        <v>254886</v>
+        <v>305297</v>
       </c>
       <c r="K285" t="inlineStr">
         <is>
@@ -14496,7 +14496,7 @@
         <v>2.22</v>
       </c>
       <c r="J287" t="n">
-        <v>95154</v>
+        <v>115553</v>
       </c>
       <c r="K287" t="inlineStr">
         <is>
@@ -14545,7 +14545,7 @@
         <v>0.14</v>
       </c>
       <c r="J288" t="n">
-        <v>965438</v>
+        <v>1082367</v>
       </c>
       <c r="K288" t="inlineStr">
         <is>
@@ -14594,7 +14594,7 @@
         <v>0.95</v>
       </c>
       <c r="J289" t="n">
-        <v>444724</v>
+        <v>593818</v>
       </c>
       <c r="K289" t="inlineStr">
         <is>
@@ -14643,7 +14643,7 @@
         <v>0.82</v>
       </c>
       <c r="J290" t="n">
-        <v>3460330</v>
+        <v>5390738</v>
       </c>
       <c r="K290" t="inlineStr">
         <is>
@@ -14741,7 +14741,7 @@
         <v>-0.19</v>
       </c>
       <c r="J292" t="n">
-        <v>2688585</v>
+        <v>3176436</v>
       </c>
       <c r="K292" t="inlineStr">
         <is>
@@ -14787,10 +14787,10 @@
         <v>127</v>
       </c>
       <c r="I293" t="n">
-        <v>-0.3</v>
+        <v>-0.23</v>
       </c>
       <c r="J293" t="n">
-        <v>2814530</v>
+        <v>2866853</v>
       </c>
       <c r="K293" t="inlineStr">
         <is>
@@ -14888,7 +14888,7 @@
         <v>0.86</v>
       </c>
       <c r="J295" t="n">
-        <v>1372963</v>
+        <v>1816441</v>
       </c>
       <c r="K295" t="inlineStr">
         <is>
@@ -14937,7 +14937,7 @@
         <v>1.28</v>
       </c>
       <c r="J296" t="n">
-        <v>1328852</v>
+        <v>1346122</v>
       </c>
       <c r="K296" t="inlineStr">
         <is>
@@ -14983,10 +14983,10 @@
         <v>52</v>
       </c>
       <c r="I297" t="n">
-        <v>0.25</v>
+        <v>0.31</v>
       </c>
       <c r="J297" t="n">
-        <v>6756544</v>
+        <v>6756878</v>
       </c>
       <c r="K297" t="inlineStr">
         <is>
@@ -15035,7 +15035,7 @@
         <v>1.65</v>
       </c>
       <c r="J298" t="n">
-        <v>807152</v>
+        <v>1020432</v>
       </c>
       <c r="K298" t="inlineStr">
         <is>
@@ -15084,7 +15084,7 @@
         <v>1.69</v>
       </c>
       <c r="J299" t="n">
-        <v>965479</v>
+        <v>1241780</v>
       </c>
       <c r="K299" t="inlineStr">
         <is>
@@ -15133,7 +15133,7 @@
         <v>0.15</v>
       </c>
       <c r="J300" t="n">
-        <v>366513</v>
+        <v>551128</v>
       </c>
       <c r="K300" t="inlineStr">
         <is>
@@ -15182,7 +15182,7 @@
         <v>0.06</v>
       </c>
       <c r="J301" t="n">
-        <v>542817</v>
+        <v>705136</v>
       </c>
       <c r="K301" t="inlineStr">
         <is>
@@ -15231,7 +15231,7 @@
         <v>1.49</v>
       </c>
       <c r="J302" t="n">
-        <v>2414184</v>
+        <v>2415722</v>
       </c>
       <c r="K302" t="inlineStr">
         <is>
@@ -15280,7 +15280,7 @@
         <v>0.31</v>
       </c>
       <c r="J303" t="n">
-        <v>2218947</v>
+        <v>2784358</v>
       </c>
       <c r="K303" t="inlineStr">
         <is>
@@ -15378,7 +15378,7 @@
         <v>0.96</v>
       </c>
       <c r="J305" t="n">
-        <v>617374</v>
+        <v>740510</v>
       </c>
       <c r="K305" t="inlineStr">
         <is>
@@ -15427,7 +15427,7 @@
         <v>-0.26</v>
       </c>
       <c r="J306" t="n">
-        <v>17524</v>
+        <v>20753</v>
       </c>
       <c r="K306" t="inlineStr">
         <is>
@@ -15571,7 +15571,7 @@
         <v>37</v>
       </c>
       <c r="I309" t="n">
-        <v>0.57</v>
+        <v>0.71</v>
       </c>
       <c r="J309" t="n">
         <v>5533335</v>
@@ -15623,7 +15623,7 @@
         <v>-0.76</v>
       </c>
       <c r="J310" t="n">
-        <v>1231538</v>
+        <v>1536211</v>
       </c>
       <c r="K310" t="inlineStr">
         <is>
@@ -15672,7 +15672,7 @@
         <v>1.23</v>
       </c>
       <c r="J311" t="n">
-        <v>1708487</v>
+        <v>1995801</v>
       </c>
       <c r="K311" t="inlineStr">
         <is>
@@ -15721,7 +15721,7 @@
         <v>1.69</v>
       </c>
       <c r="J312" t="n">
-        <v>1588084</v>
+        <v>1953396</v>
       </c>
       <c r="K312" t="inlineStr">
         <is>
@@ -15819,7 +15819,7 @@
         <v>0.67</v>
       </c>
       <c r="J314" t="n">
-        <v>1507862</v>
+        <v>1407527</v>
       </c>
       <c r="K314" t="inlineStr">
         <is>
@@ -15868,7 +15868,7 @@
         <v>1.55</v>
       </c>
       <c r="J315" t="n">
-        <v>1790948</v>
+        <v>2137543</v>
       </c>
       <c r="K315" t="inlineStr">
         <is>
@@ -15966,7 +15966,7 @@
         <v>3.85</v>
       </c>
       <c r="J317" t="n">
-        <v>363654</v>
+        <v>425195</v>
       </c>
       <c r="K317" t="inlineStr">
         <is>
@@ -16015,7 +16015,7 @@
         <v>0.77</v>
       </c>
       <c r="J318" t="n">
-        <v>170286</v>
+        <v>218093</v>
       </c>
       <c r="K318" t="inlineStr">
         <is>
@@ -16064,7 +16064,7 @@
         <v>1.59</v>
       </c>
       <c r="J319" t="n">
-        <v>864224</v>
+        <v>1129366</v>
       </c>
       <c r="K319" t="inlineStr">
         <is>
@@ -16162,7 +16162,7 @@
         <v>-2.94</v>
       </c>
       <c r="J321" t="n">
-        <v>440761</v>
+        <v>454803</v>
       </c>
       <c r="K321" t="inlineStr">
         <is>
@@ -16211,7 +16211,7 @@
         <v>0.97</v>
       </c>
       <c r="J322" t="n">
-        <v>1241295</v>
+        <v>2015424</v>
       </c>
       <c r="K322" t="inlineStr">
         <is>
@@ -16309,7 +16309,7 @@
         <v>0.37</v>
       </c>
       <c r="J324" t="n">
-        <v>949229</v>
+        <v>1221596</v>
       </c>
       <c r="K324" t="inlineStr">
         <is>
@@ -16456,7 +16456,7 @@
         <v>2.33</v>
       </c>
       <c r="J327" t="n">
-        <v>2091340</v>
+        <v>2630607</v>
       </c>
       <c r="K327" t="inlineStr">
         <is>
@@ -16603,7 +16603,7 @@
         <v>-0.84</v>
       </c>
       <c r="J330" t="n">
-        <v>916819</v>
+        <v>1183962</v>
       </c>
       <c r="K330" t="inlineStr">
         <is>
@@ -16652,7 +16652,7 @@
         <v>-0.6</v>
       </c>
       <c r="J331" t="n">
-        <v>1223130</v>
+        <v>1848453</v>
       </c>
       <c r="K331" t="inlineStr">
         <is>
@@ -16750,7 +16750,7 @@
         <v>-2.79</v>
       </c>
       <c r="J333" t="n">
-        <v>334271</v>
+        <v>454112</v>
       </c>
       <c r="K333" t="inlineStr">
         <is>
@@ -16799,7 +16799,7 @@
         <v>0.23</v>
       </c>
       <c r="J334" t="n">
-        <v>12912100</v>
+        <v>12286310</v>
       </c>
       <c r="K334" t="inlineStr">
         <is>
@@ -16848,7 +16848,7 @@
         <v>1.37</v>
       </c>
       <c r="J335" t="n">
-        <v>236757</v>
+        <v>274579</v>
       </c>
       <c r="K335" t="inlineStr">
         <is>
@@ -16946,7 +16946,7 @@
         <v>0.84</v>
       </c>
       <c r="J337" t="n">
-        <v>1387302</v>
+        <v>1688236</v>
       </c>
       <c r="K337" t="inlineStr">
         <is>
@@ -16995,7 +16995,7 @@
         <v>-0.38</v>
       </c>
       <c r="J338" t="n">
-        <v>631599</v>
+        <v>827519</v>
       </c>
       <c r="K338" t="inlineStr">
         <is>
@@ -17044,7 +17044,7 @@
         <v>0.15</v>
       </c>
       <c r="J339" t="n">
-        <v>928958</v>
+        <v>1231771</v>
       </c>
       <c r="K339" t="inlineStr">
         <is>
@@ -17093,7 +17093,7 @@
         <v>-0.18</v>
       </c>
       <c r="J340" t="n">
-        <v>1611300</v>
+        <v>2052241</v>
       </c>
       <c r="K340" t="inlineStr">
         <is>
@@ -17142,7 +17142,7 @@
         <v>-0.55</v>
       </c>
       <c r="J341" t="n">
-        <v>272934</v>
+        <v>337712</v>
       </c>
       <c r="K341" t="inlineStr">
         <is>
@@ -17240,7 +17240,7 @@
         <v>1.12</v>
       </c>
       <c r="J343" t="n">
-        <v>464335</v>
+        <v>593241</v>
       </c>
       <c r="K343" t="inlineStr">
         <is>
@@ -17286,7 +17286,7 @@
         <v>137</v>
       </c>
       <c r="I344" t="n">
-        <v>-2.19</v>
+        <v>-2.32</v>
       </c>
       <c r="J344" t="n">
         <v>1915238</v>
@@ -17387,7 +17387,7 @@
         <v>0.6</v>
       </c>
       <c r="J346" t="n">
-        <v>1406619</v>
+        <v>3549759</v>
       </c>
       <c r="K346" t="inlineStr">
         <is>
@@ -17534,7 +17534,7 @@
         <v>-0.92</v>
       </c>
       <c r="J349" t="n">
-        <v>1266609</v>
+        <v>1501184</v>
       </c>
       <c r="K349" t="inlineStr">
         <is>
@@ -17583,7 +17583,7 @@
         <v>0.38</v>
       </c>
       <c r="J350" t="n">
-        <v>231921</v>
+        <v>290164</v>
       </c>
       <c r="K350" t="inlineStr">
         <is>
@@ -17632,7 +17632,7 @@
         <v>-1.94</v>
       </c>
       <c r="J351" t="n">
-        <v>11404486</v>
+        <v>11605031</v>
       </c>
       <c r="K351" t="inlineStr">
         <is>
@@ -17681,7 +17681,7 @@
         <v>0.71</v>
       </c>
       <c r="J352" t="n">
-        <v>1378952</v>
+        <v>1757236</v>
       </c>
       <c r="K352" t="inlineStr">
         <is>
@@ -17877,7 +17877,7 @@
         <v>-2.54</v>
       </c>
       <c r="J356" t="n">
-        <v>2165776</v>
+        <v>2631709</v>
       </c>
       <c r="K356" t="inlineStr">
         <is>
@@ -17975,7 +17975,7 @@
         <v>-0.59</v>
       </c>
       <c r="J358" t="n">
-        <v>153414</v>
+        <v>218701</v>
       </c>
       <c r="K358" t="inlineStr">
         <is>
@@ -18024,7 +18024,7 @@
         <v>0.38</v>
       </c>
       <c r="J359" t="n">
-        <v>910276</v>
+        <v>1045510</v>
       </c>
       <c r="K359" t="inlineStr">
         <is>
@@ -18073,7 +18073,7 @@
         <v>-0.22</v>
       </c>
       <c r="J360" t="n">
-        <v>3774584</v>
+        <v>4700536</v>
       </c>
       <c r="K360" t="inlineStr">
         <is>
@@ -18171,7 +18171,7 @@
         <v>-0.9</v>
       </c>
       <c r="J362" t="n">
-        <v>3643534</v>
+        <v>3889378</v>
       </c>
       <c r="K362" t="inlineStr">
         <is>
@@ -18214,17 +18214,17 @@
         <v>181</v>
       </c>
       <c r="H363" t="n">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I363" t="n">
-        <v>0.9399999999999999</v>
+        <v>1.59</v>
       </c>
       <c r="J363" t="n">
-        <v>864686</v>
+        <v>866526</v>
       </c>
       <c r="K363" t="inlineStr">
         <is>
-          <t>$19.32 B</t>
+          <t>$19.45 B</t>
         </is>
       </c>
     </row>
@@ -18318,7 +18318,7 @@
         <v>1.89</v>
       </c>
       <c r="J365" t="n">
-        <v>2920641</v>
+        <v>3350118</v>
       </c>
       <c r="K365" t="inlineStr">
         <is>
@@ -18367,7 +18367,7 @@
         <v>-0.53</v>
       </c>
       <c r="J366" t="n">
-        <v>1072652</v>
+        <v>1357703</v>
       </c>
       <c r="K366" t="inlineStr">
         <is>
@@ -18416,7 +18416,7 @@
         <v>0.09</v>
       </c>
       <c r="J367" t="n">
-        <v>308887</v>
+        <v>385006</v>
       </c>
       <c r="K367" t="inlineStr">
         <is>
@@ -18465,7 +18465,7 @@
         <v>-0.64</v>
       </c>
       <c r="J368" t="n">
-        <v>1572864</v>
+        <v>2030072</v>
       </c>
       <c r="K368" t="inlineStr">
         <is>
@@ -18514,7 +18514,7 @@
         <v>0.08</v>
       </c>
       <c r="J369" t="n">
-        <v>851553</v>
+        <v>1101250</v>
       </c>
       <c r="K369" t="inlineStr">
         <is>
@@ -18563,7 +18563,7 @@
         <v>1.27</v>
       </c>
       <c r="J370" t="n">
-        <v>1450499</v>
+        <v>1674409</v>
       </c>
       <c r="K370" t="inlineStr">
         <is>
@@ -18661,7 +18661,7 @@
         <v>1.97</v>
       </c>
       <c r="J372" t="n">
-        <v>300842</v>
+        <v>423279</v>
       </c>
       <c r="K372" t="inlineStr">
         <is>
@@ -18707,7 +18707,7 @@
         <v>136</v>
       </c>
       <c r="I373" t="n">
-        <v>-1.69</v>
+        <v>-1.84</v>
       </c>
       <c r="J373" t="n">
         <v>1642539</v>
@@ -18808,7 +18808,7 @@
         <v>1.21</v>
       </c>
       <c r="J375" t="n">
-        <v>8521084</v>
+        <v>8373897</v>
       </c>
       <c r="K375" t="inlineStr">
         <is>
@@ -18857,7 +18857,7 @@
         <v>0.17</v>
       </c>
       <c r="J376" t="n">
-        <v>596840</v>
+        <v>720313</v>
       </c>
       <c r="K376" t="inlineStr">
         <is>
@@ -19053,7 +19053,7 @@
         <v>-0.24</v>
       </c>
       <c r="J380" t="n">
-        <v>175597</v>
+        <v>168117</v>
       </c>
       <c r="K380" t="inlineStr">
         <is>
@@ -19102,7 +19102,7 @@
         <v>0.37</v>
       </c>
       <c r="J381" t="n">
-        <v>416948</v>
+        <v>545873</v>
       </c>
       <c r="K381" t="inlineStr">
         <is>
@@ -19148,7 +19148,7 @@
         <v>75</v>
       </c>
       <c r="I382" t="n">
-        <v>0.53</v>
+        <v>0.64</v>
       </c>
       <c r="J382" t="n">
         <v>1189867</v>
@@ -19249,7 +19249,7 @@
         <v>0.11</v>
       </c>
       <c r="J384" t="n">
-        <v>2227086</v>
+        <v>2785373</v>
       </c>
       <c r="K384" t="inlineStr">
         <is>
@@ -19347,7 +19347,7 @@
         <v>0.14</v>
       </c>
       <c r="J386" t="n">
-        <v>301092</v>
+        <v>434217</v>
       </c>
       <c r="K386" t="inlineStr">
         <is>
@@ -19445,7 +19445,7 @@
         <v>1.41</v>
       </c>
       <c r="J388" t="n">
-        <v>819159</v>
+        <v>778399</v>
       </c>
       <c r="K388" t="inlineStr">
         <is>
@@ -19494,7 +19494,7 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="J389" t="n">
-        <v>389318</v>
+        <v>485986</v>
       </c>
       <c r="K389" t="inlineStr">
         <is>
@@ -19543,7 +19543,7 @@
         <v>-2.22</v>
       </c>
       <c r="J390" t="n">
-        <v>4662083</v>
+        <v>5520143</v>
       </c>
       <c r="K390" t="inlineStr">
         <is>
@@ -19641,7 +19641,7 @@
         <v>2.38</v>
       </c>
       <c r="J392" t="n">
-        <v>4219737</v>
+        <v>4834716</v>
       </c>
       <c r="K392" t="inlineStr">
         <is>
@@ -19690,7 +19690,7 @@
         <v>-0.45</v>
       </c>
       <c r="J393" t="n">
-        <v>361902</v>
+        <v>546977</v>
       </c>
       <c r="K393" t="inlineStr">
         <is>
@@ -19739,7 +19739,7 @@
         <v>1.14</v>
       </c>
       <c r="J394" t="n">
-        <v>2467190</v>
+        <v>2918397</v>
       </c>
       <c r="K394" t="inlineStr">
         <is>
@@ -19788,7 +19788,7 @@
         <v>-4.98</v>
       </c>
       <c r="J395" t="n">
-        <v>902103</v>
+        <v>886210</v>
       </c>
       <c r="K395" t="inlineStr">
         <is>
@@ -19837,7 +19837,7 @@
         <v>-0.28</v>
       </c>
       <c r="J396" t="n">
-        <v>7955378</v>
+        <v>9165612</v>
       </c>
       <c r="K396" t="inlineStr">
         <is>
@@ -19886,7 +19886,7 @@
         <v>2.17</v>
       </c>
       <c r="J397" t="n">
-        <v>2498311</v>
+        <v>2562074</v>
       </c>
       <c r="K397" t="inlineStr">
         <is>
@@ -19984,7 +19984,7 @@
         <v>-1.56</v>
       </c>
       <c r="J399" t="n">
-        <v>240630</v>
+        <v>356946</v>
       </c>
       <c r="K399" t="inlineStr">
         <is>
@@ -20033,7 +20033,7 @@
         <v>0.01</v>
       </c>
       <c r="J400" t="n">
-        <v>360683</v>
+        <v>456133</v>
       </c>
       <c r="K400" t="inlineStr">
         <is>
@@ -20082,7 +20082,7 @@
         <v>-0.48</v>
       </c>
       <c r="J401" t="n">
-        <v>1092177</v>
+        <v>1121378</v>
       </c>
       <c r="K401" t="inlineStr">
         <is>
@@ -20131,7 +20131,7 @@
         <v>0.82</v>
       </c>
       <c r="J402" t="n">
-        <v>1388898</v>
+        <v>1549815</v>
       </c>
       <c r="K402" t="inlineStr">
         <is>
@@ -20180,7 +20180,7 @@
         <v>-1.13</v>
       </c>
       <c r="J403" t="n">
-        <v>1010969</v>
+        <v>1100992</v>
       </c>
       <c r="K403" t="inlineStr">
         <is>
@@ -20327,7 +20327,7 @@
         <v>1.04</v>
       </c>
       <c r="J406" t="n">
-        <v>191366</v>
+        <v>280952</v>
       </c>
       <c r="K406" t="inlineStr">
         <is>
@@ -20474,7 +20474,7 @@
         <v>0.88</v>
       </c>
       <c r="J409" t="n">
-        <v>496950</v>
+        <v>613102</v>
       </c>
       <c r="K409" t="inlineStr">
         <is>
@@ -20618,7 +20618,7 @@
         <v>115</v>
       </c>
       <c r="I412" t="n">
-        <v>0.63</v>
+        <v>0.65</v>
       </c>
       <c r="J412" t="n">
         <v>3215704</v>
@@ -20670,7 +20670,7 @@
         <v>0.13</v>
       </c>
       <c r="J413" t="n">
-        <v>326421</v>
+        <v>383186</v>
       </c>
       <c r="K413" t="inlineStr">
         <is>
@@ -20768,7 +20768,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="J415" t="n">
-        <v>9513226</v>
+        <v>10217394</v>
       </c>
       <c r="K415" t="inlineStr">
         <is>
@@ -20915,7 +20915,7 @@
         <v>1.21</v>
       </c>
       <c r="J418" t="n">
-        <v>4928073</v>
+        <v>5493938</v>
       </c>
       <c r="K418" t="inlineStr">
         <is>
@@ -21111,7 +21111,7 @@
         <v>-0.18</v>
       </c>
       <c r="J422" t="n">
-        <v>953268</v>
+        <v>1145409</v>
       </c>
       <c r="K422" t="inlineStr">
         <is>
@@ -21160,7 +21160,7 @@
         <v>2.9</v>
       </c>
       <c r="J423" t="n">
-        <v>1509264</v>
+        <v>1732285</v>
       </c>
       <c r="K423" t="inlineStr">
         <is>
@@ -21356,7 +21356,7 @@
         <v>-0.89</v>
       </c>
       <c r="J427" t="n">
-        <v>2744056</v>
+        <v>3095679</v>
       </c>
       <c r="K427" t="inlineStr">
         <is>
@@ -21405,7 +21405,7 @@
         <v>1.32</v>
       </c>
       <c r="J428" t="n">
-        <v>12152129</v>
+        <v>11832088</v>
       </c>
       <c r="K428" t="inlineStr">
         <is>
@@ -21454,7 +21454,7 @@
         <v>-0.4</v>
       </c>
       <c r="J429" t="n">
-        <v>2140337</v>
+        <v>2458736</v>
       </c>
       <c r="K429" t="inlineStr">
         <is>
@@ -21552,7 +21552,7 @@
         <v>0.62</v>
       </c>
       <c r="J431" t="n">
-        <v>818075</v>
+        <v>1075623</v>
       </c>
       <c r="K431" t="inlineStr">
         <is>
@@ -21797,7 +21797,7 @@
         <v>2.28</v>
       </c>
       <c r="J436" t="n">
-        <v>1708573</v>
+        <v>2362434</v>
       </c>
       <c r="K436" t="inlineStr">
         <is>
@@ -21993,7 +21993,7 @@
         <v>1.14</v>
       </c>
       <c r="J440" t="n">
-        <v>3003294</v>
+        <v>3834108</v>
       </c>
       <c r="K440" t="inlineStr">
         <is>
@@ -22042,7 +22042,7 @@
         <v>2.93</v>
       </c>
       <c r="J441" t="n">
-        <v>2018069</v>
+        <v>2209783</v>
       </c>
       <c r="K441" t="inlineStr">
         <is>
@@ -22140,7 +22140,7 @@
         <v>1.21</v>
       </c>
       <c r="J443" t="n">
-        <v>1808521</v>
+        <v>2197652</v>
       </c>
       <c r="K443" t="inlineStr">
         <is>
@@ -22189,7 +22189,7 @@
         <v>1.18</v>
       </c>
       <c r="J444" t="n">
-        <v>3566103</v>
+        <v>4489078</v>
       </c>
       <c r="K444" t="inlineStr">
         <is>
@@ -22287,7 +22287,7 @@
         <v>0.6</v>
       </c>
       <c r="J446" t="n">
-        <v>551627</v>
+        <v>651797</v>
       </c>
       <c r="K446" t="inlineStr">
         <is>
@@ -22336,7 +22336,7 @@
         <v>-0.62</v>
       </c>
       <c r="J447" t="n">
-        <v>609729</v>
+        <v>732437</v>
       </c>
       <c r="K447" t="inlineStr">
         <is>
@@ -22532,7 +22532,7 @@
         <v>-1.43</v>
       </c>
       <c r="J451" t="n">
-        <v>1138324</v>
+        <v>1472148</v>
       </c>
       <c r="K451" t="inlineStr">
         <is>
@@ -22581,7 +22581,7 @@
         <v>0.42</v>
       </c>
       <c r="J452" t="n">
-        <v>2512081</v>
+        <v>3155274</v>
       </c>
       <c r="K452" t="inlineStr">
         <is>
@@ -22728,7 +22728,7 @@
         <v>-0.37</v>
       </c>
       <c r="J455" t="n">
-        <v>744374</v>
+        <v>847525</v>
       </c>
       <c r="K455" t="inlineStr">
         <is>
@@ -22777,7 +22777,7 @@
         <v>0.23</v>
       </c>
       <c r="J456" t="n">
-        <v>458809</v>
+        <v>530317</v>
       </c>
       <c r="K456" t="inlineStr">
         <is>
@@ -22826,7 +22826,7 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="J457" t="n">
-        <v>2264600</v>
+        <v>2913086</v>
       </c>
       <c r="K457" t="inlineStr">
         <is>
@@ -22875,7 +22875,7 @@
         <v>0.19</v>
       </c>
       <c r="J458" t="n">
-        <v>1958560</v>
+        <v>2367739</v>
       </c>
       <c r="K458" t="inlineStr">
         <is>
@@ -23022,7 +23022,7 @@
         <v>-0.39</v>
       </c>
       <c r="J461" t="n">
-        <v>547882</v>
+        <v>629642</v>
       </c>
       <c r="K461" t="inlineStr">
         <is>
@@ -23071,7 +23071,7 @@
         <v>-1.43</v>
       </c>
       <c r="J462" t="n">
-        <v>395186</v>
+        <v>432862</v>
       </c>
       <c r="K462" t="inlineStr">
         <is>
@@ -23120,7 +23120,7 @@
         <v>0.39</v>
       </c>
       <c r="J463" t="n">
-        <v>188460</v>
+        <v>221307</v>
       </c>
       <c r="K463" t="inlineStr">
         <is>
@@ -23267,7 +23267,7 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="J466" t="n">
-        <v>271919</v>
+        <v>272012</v>
       </c>
       <c r="K466" t="inlineStr">
         <is>
@@ -23365,7 +23365,7 @@
         <v>1.65</v>
       </c>
       <c r="J468" t="n">
-        <v>866002</v>
+        <v>999435</v>
       </c>
       <c r="K468" t="inlineStr">
         <is>
@@ -23414,7 +23414,7 @@
         <v>1.35</v>
       </c>
       <c r="J469" t="n">
-        <v>33341768</v>
+        <v>34464869</v>
       </c>
       <c r="K469" t="inlineStr">
         <is>
@@ -23512,7 +23512,7 @@
         <v>0.82</v>
       </c>
       <c r="J471" t="n">
-        <v>2547533</v>
+        <v>3109649</v>
       </c>
       <c r="K471" t="inlineStr">
         <is>
@@ -23610,7 +23610,7 @@
         <v>0.39</v>
       </c>
       <c r="J473" t="n">
-        <v>564410</v>
+        <v>549243</v>
       </c>
       <c r="K473" t="inlineStr">
         <is>
@@ -23708,7 +23708,7 @@
         <v>-1.79</v>
       </c>
       <c r="J475" t="n">
-        <v>954103</v>
+        <v>1115044</v>
       </c>
       <c r="K475" t="inlineStr">
         <is>
@@ -23806,7 +23806,7 @@
         <v>1.15</v>
       </c>
       <c r="J477" t="n">
-        <v>311394</v>
+        <v>300634</v>
       </c>
       <c r="K477" t="inlineStr">
         <is>
@@ -23904,7 +23904,7 @@
         <v>-0.8</v>
       </c>
       <c r="J479" t="n">
-        <v>2810724</v>
+        <v>3303608</v>
       </c>
       <c r="K479" t="inlineStr">
         <is>
@@ -24051,7 +24051,7 @@
         <v>3.63</v>
       </c>
       <c r="J482" t="n">
-        <v>178728</v>
+        <v>206043</v>
       </c>
       <c r="K482" t="inlineStr">
         <is>
@@ -24097,7 +24097,7 @@
         <v>14</v>
       </c>
       <c r="I483" t="n">
-        <v>1.23</v>
+        <v>1.09</v>
       </c>
       <c r="J483" t="n">
         <v>25455702</v>
@@ -24247,7 +24247,7 @@
         <v>-0.5600000000000001</v>
       </c>
       <c r="J486" t="n">
-        <v>275057</v>
+        <v>342240</v>
       </c>
       <c r="K486" t="inlineStr">
         <is>
@@ -24296,7 +24296,7 @@
         <v>-0.88</v>
       </c>
       <c r="J487" t="n">
-        <v>1953990</v>
+        <v>1971558</v>
       </c>
       <c r="K487" t="inlineStr">
         <is>
@@ -24345,7 +24345,7 @@
         <v>0.88</v>
       </c>
       <c r="J488" t="n">
-        <v>8696911</v>
+        <v>8588789</v>
       </c>
       <c r="K488" t="inlineStr">
         <is>
@@ -24443,7 +24443,7 @@
         <v>0.58</v>
       </c>
       <c r="J490" t="n">
-        <v>553543</v>
+        <v>741181</v>
       </c>
       <c r="K490" t="inlineStr">
         <is>
@@ -24492,7 +24492,7 @@
         <v>0.62</v>
       </c>
       <c r="J491" t="n">
-        <v>522835</v>
+        <v>669601</v>
       </c>
       <c r="K491" t="inlineStr">
         <is>
@@ -24590,7 +24590,7 @@
         <v>-0.18</v>
       </c>
       <c r="J493" t="n">
-        <v>457630</v>
+        <v>585011</v>
       </c>
       <c r="K493" t="inlineStr">
         <is>
@@ -24639,7 +24639,7 @@
         <v>-5.97</v>
       </c>
       <c r="J494" t="n">
-        <v>24985779</v>
+        <v>24999511</v>
       </c>
       <c r="K494" t="inlineStr">
         <is>
@@ -24688,7 +24688,7 @@
         <v>0.64</v>
       </c>
       <c r="J495" t="n">
-        <v>1577687</v>
+        <v>1834782</v>
       </c>
       <c r="K495" t="inlineStr">
         <is>
@@ -24737,7 +24737,7 @@
         <v>-1.48</v>
       </c>
       <c r="J496" t="n">
-        <v>2760940</v>
+        <v>2762367</v>
       </c>
       <c r="K496" t="inlineStr">
         <is>
@@ -24786,7 +24786,7 @@
         <v>1.24</v>
       </c>
       <c r="J497" t="n">
-        <v>433249</v>
+        <v>505607</v>
       </c>
       <c r="K497" t="inlineStr">
         <is>
@@ -24835,7 +24835,7 @@
         <v>3.18</v>
       </c>
       <c r="J498" t="n">
-        <v>1638789</v>
+        <v>1684718</v>
       </c>
       <c r="K498" t="inlineStr">
         <is>
@@ -24933,7 +24933,7 @@
         <v>0.57</v>
       </c>
       <c r="J500" t="n">
-        <v>848853</v>
+        <v>922412</v>
       </c>
       <c r="K500" t="inlineStr">
         <is>
@@ -24982,7 +24982,7 @@
         <v>0</v>
       </c>
       <c r="J501" t="n">
-        <v>3356234</v>
+        <v>3919455</v>
       </c>
       <c r="K501" t="inlineStr">
         <is>
@@ -25129,7 +25129,7 @@
         <v>0.48</v>
       </c>
       <c r="J504" t="n">
-        <v>4003510</v>
+        <v>4584936</v>
       </c>
       <c r="K504" t="inlineStr">
         <is>

</xml_diff>